<commit_message>
ajout du dossier projets (ppe1,ppe2,e5)
</commit_message>
<xml_diff>
--- a/public/assets/- Tableau de synthèse - Epreuve E4 - BTS SIO 2025.xlsx
+++ b/public/assets/- Tableau de synthèse - Epreuve E4 - BTS SIO 2025.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bigbenconnected0-my.sharepoint.com/personal/ymokhtari_bigben-connected_com/Documents/Bureau/IPSSI/SUPPORTS DE COURS SISR/02. 18.09.2024/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ymokhtari\portfolio\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8737F06-D2AB-4FCB-A6BF-463575143CDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{421D74D4-9EB6-49E3-9B51-33EB64E5A349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tableau de synthèse Épreuve E4" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>BTS SERVICES INFORMATIQUES AUX ORGANISATIONS</t>
   </si>
@@ -50,13 +50,7 @@
     <t xml:space="preserve">Tableau de synthèse des réalisations professionnelles </t>
   </si>
   <si>
-    <t xml:space="preserve">NOM et prénom : </t>
-  </si>
-  <si>
     <t xml:space="preserve">N° candidat : </t>
-  </si>
-  <si>
-    <t>Centre de formation :</t>
   </si>
   <si>
     <t>Option :</t>
@@ -66,9 +60,6 @@
   </si>
   <si>
     <t>▢ SLAM</t>
-  </si>
-  <si>
-    <t>Adresse URL du portfolio :</t>
   </si>
   <si>
     <t>Compétences mises en œuvre
@@ -139,6 +130,21 @@
   </si>
   <si>
     <t>Réalisations en milieu professionnel en cours de seconde année</t>
+  </si>
+  <si>
+    <t>NOM et prénom : MOKHTARI Yannis</t>
+  </si>
+  <si>
+    <t>Adresse URL du portfolio : https://mokhtari-yannis.github.io/Portfolio/</t>
+  </si>
+  <si>
+    <t>Centre de formation : IPSSI PARIS</t>
+  </si>
+  <si>
+    <t>Création d'un profile LinkedIn</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -610,7 +616,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -674,6 +680,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -757,6 +766,90 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>263982</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>163537</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>457667</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>371202</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Supérieure 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7FAA1AF8-BAE4-40A7-8AD6-B0CAF4538DC0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="2868933">
+          <a:off x="11150710" y="1693993"/>
+          <a:ext cx="207665" cy="193685"/>
+        </a:xfrm>
+        <a:prstGeom prst="mathPlus">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 3680"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="000000"/>
+        </a:solidFill>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:srgbClr val="FFFFFF"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-lt"/>
+            <a:cs typeface="+mn-lt"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1051,138 +1144,138 @@
   </sheetPr>
   <dimension ref="A1:AQ81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:E3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="46" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.90625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="70.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.88671875" style="1" customWidth="1"/>
-    <col min="3" max="8" width="18.6640625" style="1" customWidth="1"/>
-    <col min="9" max="43" width="11.44140625" customWidth="1"/>
-    <col min="44" max="16384" width="10.88671875" style="1"/>
+    <col min="1" max="1" width="70.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.90625" style="1" customWidth="1"/>
+    <col min="3" max="8" width="18.6328125" style="1" customWidth="1"/>
+    <col min="9" max="43" width="11.453125" customWidth="1"/>
+    <col min="44" max="16384" width="10.90625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="22"/>
-    </row>
-    <row r="2" spans="1:43" ht="41.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="22" t="s">
+      <c r="H1" s="23"/>
+    </row>
+    <row r="2" spans="1:43" ht="41.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
     </row>
     <row r="3" spans="1:43" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" s="24"/>
-      <c r="H3" s="30"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="31"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="12" t="s">
+      <c r="H4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="13" t="s">
+    </row>
+    <row r="5" spans="1:43" ht="39.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="43"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="44"/>
+    </row>
+    <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="B6" s="40" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:43" ht="39.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="41" t="s">
+      <c r="C6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="42"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="43"/>
-    </row>
-    <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
+      <c r="D6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="39" t="s">
+      <c r="E6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="F6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="G6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="H6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="6" t="s">
+    </row>
+    <row r="7" spans="1:43" s="2" customFormat="1" ht="324.89999999999998" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="33"/>
+      <c r="B7" s="41"/>
+      <c r="C7" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="D7" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="E7" s="20" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:43" s="2" customFormat="1" ht="324.89999999999998" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="32"/>
-      <c r="B7" s="40"/>
-      <c r="C7" s="20" t="s">
+      <c r="F7" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="G7" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="H7" s="21" t="s">
         <v>20</v>
-      </c>
-      <c r="F7" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" s="21" t="s">
-        <v>23</v>
       </c>
       <c r="I7"/>
       <c r="J7"/>
@@ -1220,17 +1313,17 @@
       <c r="AP7"/>
       <c r="AQ7"/>
     </row>
-    <row r="8" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A8" s="33" t="s">
-        <v>24</v>
+    <row r="8" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A8" s="34" t="s">
+        <v>21</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="35"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="36"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1673,14 +1766,18 @@
       <c r="AQ17"/>
     </row>
     <row r="18" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
+      <c r="A18" s="9" t="s">
+        <v>27</v>
+      </c>
       <c r="B18" s="8"/>
       <c r="C18" s="15"/>
       <c r="D18" s="15"/>
       <c r="E18" s="15"/>
       <c r="F18" s="15"/>
       <c r="G18" s="15"/>
-      <c r="H18" s="16"/>
+      <c r="H18" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="I18"/>
       <c r="J18"/>
       <c r="K18"/>
@@ -1717,17 +1814,17 @@
       <c r="AP18"/>
       <c r="AQ18"/>
     </row>
-    <row r="19" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A19" s="36" t="s">
-        <v>25</v>
+    <row r="19" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A19" s="37" t="s">
+        <v>22</v>
       </c>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="37"/>
-      <c r="H19" s="38"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="39"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -2079,17 +2176,17 @@
       <c r="AP26"/>
       <c r="AQ26"/>
     </row>
-    <row r="27" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A27" s="36" t="s">
-        <v>26</v>
+    <row r="27" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A27" s="37" t="s">
+        <v>23</v>
       </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="38"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="39"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2441,7 +2538,7 @@
       <c r="AP34"/>
       <c r="AQ34"/>
     </row>
-    <row r="35" spans="1:43" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:43" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
       <c r="B35" s="3"/>
       <c r="C35" s="4"/>
@@ -2552,6 +2649,7 @@
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup paperSize="9" scale="48" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
tbs ; doc veille ; schéma réseau
</commit_message>
<xml_diff>
--- a/public/assets/- Tableau de synthèse - Epreuve E4 - BTS SIO 2025.xlsx
+++ b/public/assets/- Tableau de synthèse - Epreuve E4 - BTS SIO 2025.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ymokhtari\portfolio\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4693D55D-E872-48ED-AF62-022E9149F487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A89F7312-A603-4EB9-903C-F1AB1944DFA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="11370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tableau de synthèse Épreuve E4" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Tableau de synthèse Épreuve E4'!$A$1:$H$35</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Tableau de synthèse Épreuve E4'!$A$1:$H$30</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="54">
   <si>
     <t>BTS SERVICES INFORMATIQUES AUX ORGANISATIONS</t>
   </si>
@@ -154,6 +154,72 @@
   </si>
   <si>
     <t>du 02/09/2024 au 18/07/2025</t>
+  </si>
+  <si>
+    <t>Creation d'entreprise virtuelle (AP1)</t>
+  </si>
+  <si>
+    <t>Installation et configuration d'un Hyperviseur Proxmox VE</t>
+  </si>
+  <si>
+    <t>du 30/09/2024 au 14/10/2024</t>
+  </si>
+  <si>
+    <t>Mise une place d'une Machine Virtuel (Windows, Linux)</t>
+  </si>
+  <si>
+    <t>Installation et configuration d’un outil d’inventaire et ticketing (GLPI)</t>
+  </si>
+  <si>
+    <t>Mettre en place un outil de veille technologique (Feedly, Google Alerts)</t>
+  </si>
+  <si>
+    <t>du 19/10/2024 au 02/11/2024</t>
+  </si>
+  <si>
+    <t>Création d'un portfolio avec Astro (sur base de template)</t>
+  </si>
+  <si>
+    <t>Répondre aux problématique M2L (AP2)</t>
+  </si>
+  <si>
+    <t>du XX/XX/XXXX au XX/XX/XXXX</t>
+  </si>
+  <si>
+    <t>Gestion des utilisateurs dans l’Active Directory</t>
+  </si>
+  <si>
+    <t>Installation et configurations de postes pour les utilisateurs</t>
+  </si>
+  <si>
+    <t>Installation et configuration d'un Windows serveur 2022 AD</t>
+  </si>
+  <si>
+    <t>du 28/10/2024 au 04/11/2024</t>
+  </si>
+  <si>
+    <t>du 08/09/2024 au XX/XX/XXXX</t>
+  </si>
+  <si>
+    <t>Mise à jour de GLPI vers la version la plus récente + configuration</t>
+  </si>
+  <si>
+    <t>Création d'un cron pour les actions automatiques GLPI</t>
+  </si>
+  <si>
+    <t>Assistance aux utilisateurs</t>
+  </si>
+  <si>
+    <t>Installation et brassage des prises RJ45</t>
+  </si>
+  <si>
+    <t>Inventaire du matériel informatique</t>
+  </si>
+  <si>
+    <t>Création de documents techniques</t>
+  </si>
+  <si>
+    <t>Installation d'un serveur mail (Postfix)</t>
   </si>
 </sst>
 </file>
@@ -163,7 +229,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-1]_-;\-* #,##0.00\ [$€-1]_-;_-* &quot;-&quot;??\ [$€-1]_-"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -225,6 +291,26 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -234,7 +320,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -620,12 +706,57 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -633,15 +764,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -687,36 +809,48 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -755,6 +889,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1148,139 +1285,139 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AQ81"/>
+  <dimension ref="A1:AQ76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="50" zoomScaleNormal="400" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.90625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="70.453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="29.26953125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="41.81640625" style="1" customWidth="1"/>
     <col min="3" max="8" width="18.6328125" style="1" customWidth="1"/>
     <col min="9" max="43" width="11.453125" customWidth="1"/>
     <col min="44" max="16384" width="10.90625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24" t="s">
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="24"/>
+      <c r="H1" s="25"/>
     </row>
     <row r="2" spans="1:43" ht="41.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
     </row>
     <row r="3" spans="1:43" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="42" t="s">
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="37"/>
-      <c r="H3" s="43"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="44"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="11" t="s">
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="H4" s="15" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="39.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="35"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="36"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="H6" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="324.89999999999998" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="23"/>
-      <c r="B7" s="32"/>
-      <c r="C7" s="19" t="s">
+      <c r="A7" s="24"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="E7" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="19" t="s">
+      <c r="F7" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="19" t="s">
+      <c r="G7" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="20" t="s">
+      <c r="H7" s="17" t="s">
         <v>20</v>
       </c>
       <c r="I7"/>
@@ -1320,16 +1457,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="27"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="28"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1366,15 +1503,23 @@
       <c r="AP8"/>
       <c r="AQ8"/>
     </row>
-    <row r="9" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="15"/>
+    <row r="9" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A9" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="11"/>
+      <c r="H9" s="12"/>
       <c r="I9"/>
       <c r="J9"/>
       <c r="K9"/>
@@ -1411,15 +1556,23 @@
       <c r="AP9"/>
       <c r="AQ9"/>
     </row>
-    <row r="10" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="15"/>
+    <row r="10" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A10" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10" s="12"/>
       <c r="I10"/>
       <c r="J10"/>
       <c r="K10"/>
@@ -1456,15 +1609,25 @@
       <c r="AP10"/>
       <c r="AQ10"/>
     </row>
-    <row r="11" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="15"/>
+    <row r="11" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A11" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" s="12"/>
       <c r="I11"/>
       <c r="J11"/>
       <c r="K11"/>
@@ -1501,15 +1664,23 @@
       <c r="AP11"/>
       <c r="AQ11"/>
     </row>
-    <row r="12" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="15"/>
+    <row r="12" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A12" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="H12" s="12"/>
       <c r="I12"/>
       <c r="J12"/>
       <c r="K12"/>
@@ -1546,15 +1717,21 @@
       <c r="AP12"/>
       <c r="AQ12"/>
     </row>
-    <row r="13" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="15"/>
+    <row r="13" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A13" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" s="11"/>
+      <c r="H13" s="12"/>
       <c r="I13"/>
       <c r="J13"/>
       <c r="K13"/>
@@ -1591,15 +1768,19 @@
       <c r="AP13"/>
       <c r="AQ13"/>
     </row>
-    <row r="14" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="15"/>
+    <row r="14" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A14" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="12"/>
       <c r="I14"/>
       <c r="J14"/>
       <c r="K14"/>
@@ -1636,15 +1817,23 @@
       <c r="AP14"/>
       <c r="AQ14"/>
     </row>
-    <row r="15" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="15"/>
+    <row r="15" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A15" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="11"/>
+      <c r="D15" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="H15" s="12"/>
       <c r="I15"/>
       <c r="J15"/>
       <c r="K15"/>
@@ -1681,15 +1870,23 @@
       <c r="AP15"/>
       <c r="AQ15"/>
     </row>
-    <row r="16" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="15"/>
+    <row r="16" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A16" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="I16"/>
       <c r="J16"/>
       <c r="K16"/>
@@ -1727,14 +1924,20 @@
       <c r="AQ16"/>
     </row>
     <row r="17" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="15"/>
+      <c r="A17" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="19" t="s">
+        <v>28</v>
+      </c>
       <c r="I17"/>
       <c r="J17"/>
       <c r="K17"/>
@@ -1772,18 +1975,18 @@
       <c r="AQ17"/>
     </row>
     <row r="18" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="21" t="s">
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="19" t="s">
         <v>28</v>
       </c>
       <c r="I18"/>
@@ -1823,16 +2026,16 @@
       <c r="AQ18"/>
     </row>
     <row r="19" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A19" s="28" t="s">
+      <c r="A19" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="29"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="30"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="30"/>
+      <c r="H19" s="31"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -1869,17 +2072,21 @@
       <c r="AP19"/>
       <c r="AQ19"/>
     </row>
-    <row r="20" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="9"/>
-      <c r="B20" s="8" t="s">
+    <row r="20" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A20" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="15"/>
+      <c r="C20" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="12"/>
       <c r="I20"/>
       <c r="J20"/>
       <c r="K20"/>
@@ -1916,17 +2123,23 @@
       <c r="AP20"/>
       <c r="AQ20"/>
     </row>
-    <row r="21" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="9"/>
-      <c r="B21" s="8" t="s">
+    <row r="21" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A21" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="15"/>
+      <c r="C21" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="12"/>
       <c r="I21"/>
       <c r="J21"/>
       <c r="K21"/>
@@ -1963,17 +2176,19 @@
       <c r="AP21"/>
       <c r="AQ21"/>
     </row>
-    <row r="22" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="9"/>
-      <c r="B22" s="8" t="s">
+    <row r="22" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A22" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="15"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="12"/>
       <c r="I22"/>
       <c r="J22"/>
       <c r="K22"/>
@@ -2011,16 +2226,18 @@
       <c r="AQ22"/>
     </row>
     <row r="23" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="9"/>
-      <c r="B23" s="8" t="s">
+      <c r="A23" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="15"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="12"/>
       <c r="I23"/>
       <c r="J23"/>
       <c r="K23"/>
@@ -2057,17 +2274,15 @@
       <c r="AP23"/>
       <c r="AQ23"/>
     </row>
-    <row r="24" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="9"/>
-      <c r="B24" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="15"/>
+    <row r="24" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A24" s="6"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="12"/>
       <c r="I24"/>
       <c r="J24"/>
       <c r="K24"/>
@@ -2104,17 +2319,17 @@
       <c r="AP24"/>
       <c r="AQ24"/>
     </row>
-    <row r="25" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="9"/>
-      <c r="B25" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="15"/>
+    <row r="25" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A25" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="30"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="30"/>
+      <c r="H25" s="31"/>
       <c r="I25"/>
       <c r="J25"/>
       <c r="K25"/>
@@ -2151,17 +2366,23 @@
       <c r="AP25"/>
       <c r="AQ25"/>
     </row>
-    <row r="26" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="9"/>
-      <c r="B26" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="15"/>
+    <row r="26" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A26" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="12"/>
       <c r="I26"/>
       <c r="J26"/>
       <c r="K26"/>
@@ -2198,17 +2419,19 @@
       <c r="AP26"/>
       <c r="AQ26"/>
     </row>
-    <row r="27" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A27" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="B27" s="29"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="29"/>
-      <c r="H27" s="30"/>
+    <row r="27" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="12"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2245,17 +2468,19 @@
       <c r="AP27"/>
       <c r="AQ27"/>
     </row>
-    <row r="28" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="9"/>
-      <c r="B28" s="8" t="s">
+    <row r="28" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A28" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="15"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="12"/>
       <c r="I28"/>
       <c r="J28"/>
       <c r="K28"/>
@@ -2292,17 +2517,23 @@
       <c r="AP28"/>
       <c r="AQ28"/>
     </row>
-    <row r="29" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="9"/>
-      <c r="B29" s="8" t="s">
+    <row r="29" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A29" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="15"/>
+      <c r="C29" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29" s="18"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="H29" s="12"/>
       <c r="I29"/>
       <c r="J29"/>
       <c r="K29"/>
@@ -2339,17 +2570,15 @@
       <c r="AP29"/>
       <c r="AQ29"/>
     </row>
-    <row r="30" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="9"/>
-      <c r="B30" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="15"/>
+    <row r="30" spans="1:43" s="2" customFormat="1" ht="30.5" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="A30" s="7"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="14"/>
       <c r="I30"/>
       <c r="J30"/>
       <c r="K30"/>
@@ -2386,252 +2615,24 @@
       <c r="AP30"/>
       <c r="AQ30"/>
     </row>
-    <row r="31" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="9"/>
-      <c r="B31" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="15"/>
-      <c r="I31"/>
-      <c r="J31"/>
-      <c r="K31"/>
-      <c r="L31"/>
-      <c r="M31"/>
-      <c r="N31"/>
-      <c r="O31"/>
-      <c r="P31"/>
-      <c r="Q31"/>
-      <c r="R31"/>
-      <c r="S31"/>
-      <c r="T31"/>
-      <c r="U31"/>
-      <c r="V31"/>
-      <c r="W31"/>
-      <c r="X31"/>
-      <c r="Y31"/>
-      <c r="Z31"/>
-      <c r="AA31"/>
-      <c r="AB31"/>
-      <c r="AC31"/>
-      <c r="AD31"/>
-      <c r="AE31"/>
-      <c r="AF31"/>
-      <c r="AG31"/>
-      <c r="AH31"/>
-      <c r="AI31"/>
-      <c r="AJ31"/>
-      <c r="AK31"/>
-      <c r="AL31"/>
-      <c r="AM31"/>
-      <c r="AN31"/>
-      <c r="AO31"/>
-      <c r="AP31"/>
-      <c r="AQ31"/>
-    </row>
-    <row r="32" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="9"/>
-      <c r="B32" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="15"/>
-      <c r="I32"/>
-      <c r="J32"/>
-      <c r="K32"/>
-      <c r="L32"/>
-      <c r="M32"/>
-      <c r="N32"/>
-      <c r="O32"/>
-      <c r="P32"/>
-      <c r="Q32"/>
-      <c r="R32"/>
-      <c r="S32"/>
-      <c r="T32"/>
-      <c r="U32"/>
-      <c r="V32"/>
-      <c r="W32"/>
-      <c r="X32"/>
-      <c r="Y32"/>
-      <c r="Z32"/>
-      <c r="AA32"/>
-      <c r="AB32"/>
-      <c r="AC32"/>
-      <c r="AD32"/>
-      <c r="AE32"/>
-      <c r="AF32"/>
-      <c r="AG32"/>
-      <c r="AH32"/>
-      <c r="AI32"/>
-      <c r="AJ32"/>
-      <c r="AK32"/>
-      <c r="AL32"/>
-      <c r="AM32"/>
-      <c r="AN32"/>
-      <c r="AO32"/>
-      <c r="AP32"/>
-      <c r="AQ32"/>
-    </row>
-    <row r="33" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="9"/>
-      <c r="B33" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C33" s="14"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="15"/>
-      <c r="I33"/>
-      <c r="J33"/>
-      <c r="K33"/>
-      <c r="L33"/>
-      <c r="M33"/>
-      <c r="N33"/>
-      <c r="O33"/>
-      <c r="P33"/>
-      <c r="Q33"/>
-      <c r="R33"/>
-      <c r="S33"/>
-      <c r="T33"/>
-      <c r="U33"/>
-      <c r="V33"/>
-      <c r="W33"/>
-      <c r="X33"/>
-      <c r="Y33"/>
-      <c r="Z33"/>
-      <c r="AA33"/>
-      <c r="AB33"/>
-      <c r="AC33"/>
-      <c r="AD33"/>
-      <c r="AE33"/>
-      <c r="AF33"/>
-      <c r="AG33"/>
-      <c r="AH33"/>
-      <c r="AI33"/>
-      <c r="AJ33"/>
-      <c r="AK33"/>
-      <c r="AL33"/>
-      <c r="AM33"/>
-      <c r="AN33"/>
-      <c r="AO33"/>
-      <c r="AP33"/>
-      <c r="AQ33"/>
-    </row>
-    <row r="34" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="10"/>
-      <c r="B34" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C34" s="16"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="16"/>
-      <c r="H34" s="17"/>
-      <c r="I34"/>
-      <c r="J34"/>
-      <c r="K34"/>
-      <c r="L34"/>
-      <c r="M34"/>
-      <c r="N34"/>
-      <c r="O34"/>
-      <c r="P34"/>
-      <c r="Q34"/>
-      <c r="R34"/>
-      <c r="S34"/>
-      <c r="T34"/>
-      <c r="U34"/>
-      <c r="V34"/>
-      <c r="W34"/>
-      <c r="X34"/>
-      <c r="Y34"/>
-      <c r="Z34"/>
-      <c r="AA34"/>
-      <c r="AB34"/>
-      <c r="AC34"/>
-      <c r="AD34"/>
-      <c r="AE34"/>
-      <c r="AF34"/>
-      <c r="AG34"/>
-      <c r="AH34"/>
-      <c r="AI34"/>
-      <c r="AJ34"/>
-      <c r="AK34"/>
-      <c r="AL34"/>
-      <c r="AM34"/>
-      <c r="AN34"/>
-      <c r="AO34"/>
-      <c r="AP34"/>
-      <c r="AQ34"/>
-    </row>
-    <row r="35" spans="1:43" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.25">
-      <c r="A35" s="5"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-      <c r="I35"/>
-      <c r="J35"/>
-      <c r="K35"/>
-      <c r="L35"/>
-      <c r="M35"/>
-      <c r="N35"/>
-      <c r="O35"/>
-      <c r="P35"/>
-      <c r="Q35"/>
-      <c r="R35"/>
-      <c r="S35"/>
-      <c r="T35"/>
-      <c r="U35"/>
-      <c r="V35"/>
-      <c r="W35"/>
-      <c r="X35"/>
-      <c r="Y35"/>
-      <c r="Z35"/>
-      <c r="AA35"/>
-      <c r="AB35"/>
-      <c r="AC35"/>
-      <c r="AD35"/>
-      <c r="AE35"/>
-      <c r="AF35"/>
-      <c r="AG35"/>
-      <c r="AH35"/>
-      <c r="AI35"/>
-      <c r="AJ35"/>
-      <c r="AK35"/>
-      <c r="AL35"/>
-      <c r="AM35"/>
-      <c r="AN35"/>
-      <c r="AO35"/>
-      <c r="AP35"/>
-      <c r="AQ35"/>
-    </row>
-    <row r="36" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="49" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="50" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="51" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -2660,11 +2661,6 @@
     <row r="74" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="75" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="76" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="77" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="78" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="79" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="80" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="81" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
     <mergeCell ref="G1:H1"/>
@@ -2676,16 +2672,16 @@
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
     <mergeCell ref="A19:H19"/>
-    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="A25:H25"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0.51181102362204722" footer="0.51181102362204722"/>
-  <pageSetup paperSize="9" scale="48" orientation="portrait"/>
+  <pageSetup paperSize="9" scale="46" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
changement image contact attestation profil + maj-documentations
</commit_message>
<xml_diff>
--- a/public/assets/- Tableau de synthèse - Epreuve E4 - BTS SIO 2025.xlsx
+++ b/public/assets/- Tableau de synthèse - Epreuve E4 - BTS SIO 2025.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ymokhtari\portfolio\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E177735-9930-4A16-8357-D73398D354AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D2E785D-ADDC-47F5-B38C-3C81826D8442}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -216,10 +216,10 @@
     <t>Mise une place d'une Machine Virtuelle (Windows, Linux)</t>
   </si>
   <si>
-    <t>Installation d'un serveur mail (Zimbra)</t>
-  </si>
-  <si>
     <t>N° candidat : 02444882291</t>
+  </si>
+  <si>
+    <t>Installation d'un serveur mail (iRedMail)</t>
   </si>
 </sst>
 </file>
@@ -827,15 +827,39 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -867,30 +891,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1287,8 +1287,8 @@
   </sheetPr>
   <dimension ref="A1:AQ76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="400" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="68" zoomScaleNormal="400" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.90625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1301,56 +1301,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="26"/>
+      <c r="H1" s="24"/>
     </row>
     <row r="2" spans="1:43" ht="41.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
     </row>
     <row r="3" spans="1:43" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="G3" s="39"/>
-      <c r="H3" s="45"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" s="26"/>
+      <c r="H3" s="32"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="43"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="30"/>
       <c r="F4" s="8" t="s">
         <v>3</v>
       </c>
@@ -1362,22 +1362,22 @@
       </c>
     </row>
     <row r="5" spans="1:43" ht="39.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="37"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="45"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="41" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -1400,8 +1400,8 @@
       </c>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="324.89999999999998" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="25"/>
-      <c r="B7" s="34"/>
+      <c r="A7" s="34"/>
+      <c r="B7" s="42"/>
       <c r="C7" s="16" t="s">
         <v>14</v>
       </c>
@@ -1457,16 +1457,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="29"/>
+      <c r="B8" s="36"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="37"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1770,7 +1770,7 @@
     </row>
     <row r="14" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A14" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>39</v>
@@ -2026,16 +2026,16 @@
       <c r="AQ18"/>
     </row>
     <row r="19" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A19" s="30" t="s">
+      <c r="A19" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="31"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="32"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="40"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -2320,16 +2320,16 @@
       <c r="AQ24"/>
     </row>
     <row r="25" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A25" s="30" t="s">
+      <c r="A25" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="31"/>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="31"/>
-      <c r="G25" s="31"/>
-      <c r="H25" s="32"/>
+      <c r="B25" s="39"/>
+      <c r="C25" s="39"/>
+      <c r="D25" s="39"/>
+      <c r="E25" s="39"/>
+      <c r="F25" s="39"/>
+      <c r="G25" s="39"/>
+      <c r="H25" s="40"/>
       <c r="I25"/>
       <c r="J25"/>
       <c r="K25"/>
@@ -2663,11 +2663,6 @@
     <row r="76" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
@@ -2675,6 +2670,11 @@
     <mergeCell ref="A25:H25"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -2686,6 +2686,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="33be216a-8dce-4221-a6bf-8c36a3d06712">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="1171238c-1b54-43cc-8131-966ae2953e77" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E1DC78E791988D4F8F27D6461D63FA16" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2d78a8b2e0a2ca160b65eaa5e9a9d28a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="33be216a-8dce-4221-a6bf-8c36a3d06712" xmlns:ns3="1171238c-1b54-43cc-8131-966ae2953e77" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="561b3d998887e548b368329c13219ab3" ns2:_="" ns3:_="">
     <xsd:import namespace="33be216a-8dce-4221-a6bf-8c36a3d06712"/>
@@ -2880,27 +2900,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="33be216a-8dce-4221-a6bf-8c36a3d06712">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="1171238c-1b54-43cc-8131-966ae2953e77" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63C66942-CF74-458B-BC10-322C618404A1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{162AC446-29F6-474F-810E-9BB057397515}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="33be216a-8dce-4221-a6bf-8c36a3d06712"/>
+    <ds:schemaRef ds:uri="1171238c-1b54-43cc-8131-966ae2953e77"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2C37A6B-F80B-4373-B955-1C9E4F79A7B6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2917,23 +2936,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{162AC446-29F6-474F-810E-9BB057397515}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="33be216a-8dce-4221-a6bf-8c36a3d06712"/>
-    <ds:schemaRef ds:uri="1171238c-1b54-43cc-8131-966ae2953e77"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63C66942-CF74-458B-BC10-322C618404A1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
documentation ajout de sources veille techno
</commit_message>
<xml_diff>
--- a/public/assets/- Tableau de synthèse - Epreuve E4 - BTS SIO 2025.xlsx
+++ b/public/assets/- Tableau de synthèse - Epreuve E4 - BTS SIO 2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ymokhtari\portfolio\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D2E785D-ADDC-47F5-B38C-3C81826D8442}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D0395C7-7B0A-47EE-9A42-ADEF550396E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Tableau de synthèse Épreuve E4" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Tableau de synthèse Épreuve E4'!$A$1:$H$30</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Tableau de synthèse Épreuve E4'!$A$1:$H$29</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="52">
   <si>
     <t>BTS SERVICES INFORMATIQUES AUX ORGANISATIONS</t>
   </si>
@@ -171,9 +171,6 @@
     <t>du 19/10/2024 au 02/11/2024</t>
   </si>
   <si>
-    <t>Création d'un portfolio avec Astro (sur base de template)</t>
-  </si>
-  <si>
     <t>Répondre aux problématique M2L (AP2)</t>
   </si>
   <si>
@@ -192,12 +189,6 @@
     <t>du 28/10/2024 au 04/11/2024</t>
   </si>
   <si>
-    <t>du 08/09/2024 au XX/XX/XXXX</t>
-  </si>
-  <si>
-    <t>Mise à jour de GLPI vers la version la plus récente + configuration</t>
-  </si>
-  <si>
     <t>Création d'un cron pour les actions automatiques GLPI</t>
   </si>
   <si>
@@ -207,12 +198,6 @@
     <t>Installation et brassage des prises RJ45</t>
   </si>
   <si>
-    <t>Inventaire du matériel informatique</t>
-  </si>
-  <si>
-    <t>Création de documents techniques</t>
-  </si>
-  <si>
     <t>Mise une place d'une Machine Virtuelle (Windows, Linux)</t>
   </si>
   <si>
@@ -220,6 +205,15 @@
   </si>
   <si>
     <t>Installation d'un serveur mail (iRedMail)</t>
+  </si>
+  <si>
+    <t>Mise à jour de GLPI vers la version la plus récente + configuration du profil</t>
+  </si>
+  <si>
+    <t>Implantation d'une GPO logiciel (Group Policy Object)</t>
+  </si>
+  <si>
+    <t>Import/Export des listes d'adresses via l'interface web de l'imprimante</t>
   </si>
 </sst>
 </file>
@@ -320,7 +314,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -725,21 +719,6 @@
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -756,7 +735,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -815,16 +794,13 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1285,10 +1261,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AQ76"/>
+  <dimension ref="A1:AQ75"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="68" zoomScaleNormal="400" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.90625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1301,56 +1277,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="24"/>
+      <c r="H1" s="23"/>
     </row>
     <row r="2" spans="1:43" ht="41.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
     </row>
     <row r="3" spans="1:43" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="31" t="s">
-        <v>52</v>
-      </c>
-      <c r="G3" s="26"/>
-      <c r="H3" s="32"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" s="25"/>
+      <c r="H3" s="31"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="30"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="29"/>
       <c r="F4" s="8" t="s">
         <v>3</v>
       </c>
@@ -1362,22 +1338,22 @@
       </c>
     </row>
     <row r="5" spans="1:43" ht="39.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="44"/>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="45"/>
+      <c r="B5" s="43"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="44"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="40" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -1400,8 +1376,8 @@
       </c>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="324.89999999999998" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="34"/>
-      <c r="B7" s="42"/>
+      <c r="A7" s="33"/>
+      <c r="B7" s="41"/>
       <c r="C7" s="16" t="s">
         <v>14</v>
       </c>
@@ -1457,16 +1433,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="36"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="37"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="36"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1508,7 +1484,7 @@
         <v>31</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="11"/>
@@ -1558,20 +1534,18 @@
     </row>
     <row r="10" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A10" s="6" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>27</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="C10" s="11"/>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="18" t="s">
+      <c r="F10" s="18" t="s">
         <v>27</v>
       </c>
+      <c r="G10" s="11"/>
       <c r="H10" s="12"/>
       <c r="I10"/>
       <c r="J10"/>
@@ -1611,10 +1585,10 @@
     </row>
     <row r="11" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A11" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C11" s="18" t="s">
         <v>27</v>
@@ -1666,10 +1640,10 @@
     </row>
     <row r="12" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A12" s="6" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C12" s="18" t="s">
         <v>27</v>
@@ -1719,18 +1693,20 @@
     </row>
     <row r="13" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A13" s="6" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="11"/>
+        <v>33</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
-      <c r="F13" s="18" t="s">
+      <c r="F13" s="11"/>
+      <c r="G13" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="G13" s="11"/>
       <c r="H13" s="12"/>
       <c r="I13"/>
       <c r="J13"/>
@@ -1770,10 +1746,10 @@
     </row>
     <row r="14" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A14" s="6" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C14" s="18"/>
       <c r="D14" s="18"/>
@@ -1822,7 +1798,7 @@
         <v>34</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="18" t="s">
@@ -1830,7 +1806,7 @@
       </c>
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
-      <c r="G15" s="21" t="s">
+      <c r="G15" s="20" t="s">
         <v>27</v>
       </c>
       <c r="H15" s="12"/>
@@ -1870,21 +1846,19 @@
       <c r="AP15"/>
       <c r="AQ15"/>
     </row>
-    <row r="16" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="16" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
-      <c r="E16" s="18" t="s">
-        <v>27</v>
-      </c>
+      <c r="E16" s="11"/>
       <c r="F16" s="11"/>
       <c r="G16" s="11"/>
-      <c r="H16" s="20" t="s">
+      <c r="H16" s="19" t="s">
         <v>27</v>
       </c>
       <c r="I16"/>
@@ -1925,10 +1899,10 @@
     </row>
     <row r="17" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C17" s="11"/>
       <c r="D17" s="11"/>
@@ -1974,21 +1948,17 @@
       <c r="AP17"/>
       <c r="AQ17"/>
     </row>
-    <row r="18" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="19" t="s">
-        <v>27</v>
-      </c>
+    <row r="18" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A18" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="38"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="39"/>
       <c r="I18"/>
       <c r="J18"/>
       <c r="K18"/>
@@ -2025,17 +1995,21 @@
       <c r="AP18"/>
       <c r="AQ18"/>
     </row>
-    <row r="19" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A19" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="39"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="40"/>
+    <row r="19" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A19" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="12"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -2074,7 +2048,7 @@
     </row>
     <row r="20" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A20" s="6" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>29</v>
@@ -2082,7 +2056,9 @@
       <c r="C20" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="11"/>
+      <c r="D20" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>
       <c r="G20" s="11"/>
@@ -2125,17 +2101,13 @@
     </row>
     <row r="21" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A21" s="6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="D21" s="18" t="s">
-        <v>27</v>
-      </c>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
       <c r="E21" s="11"/>
       <c r="F21" s="11"/>
       <c r="G21" s="11"/>
@@ -2176,15 +2148,15 @@
       <c r="AP21"/>
       <c r="AQ21"/>
     </row>
-    <row r="22" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="22" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
       <c r="E22" s="11"/>
       <c r="F22" s="11"/>
       <c r="G22" s="11"/>
@@ -2225,15 +2197,11 @@
       <c r="AP22"/>
       <c r="AQ22"/>
     </row>
-    <row r="23" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
+    <row r="23" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A23" s="6"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
       <c r="E23" s="11"/>
       <c r="F23" s="11"/>
       <c r="G23" s="11"/>
@@ -2274,15 +2242,17 @@
       <c r="AP23"/>
       <c r="AQ23"/>
     </row>
-    <row r="24" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A24" s="6"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="12"/>
+    <row r="24" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A24" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="38"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="39"/>
       <c r="I24"/>
       <c r="J24"/>
       <c r="K24"/>
@@ -2319,17 +2289,23 @@
       <c r="AP24"/>
       <c r="AQ24"/>
     </row>
-    <row r="25" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A25" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="B25" s="39"/>
-      <c r="C25" s="39"/>
-      <c r="D25" s="39"/>
-      <c r="E25" s="39"/>
-      <c r="F25" s="39"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="40"/>
+    <row r="25" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A25" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="12"/>
       <c r="I25"/>
       <c r="J25"/>
       <c r="K25"/>
@@ -2368,7 +2344,7 @@
     </row>
     <row r="26" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A26" s="6" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>30</v>
@@ -2376,12 +2352,12 @@
       <c r="C26" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D26" s="18" t="s">
-        <v>27</v>
-      </c>
+      <c r="D26" s="18"/>
       <c r="E26" s="11"/>
       <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
+      <c r="G26" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="H26" s="12"/>
       <c r="I26"/>
       <c r="J26"/>
@@ -2419,18 +2395,18 @@
       <c r="AP26"/>
       <c r="AQ26"/>
     </row>
-    <row r="27" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A27" s="6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="11"/>
+      <c r="C27" s="18"/>
       <c r="D27" s="11"/>
       <c r="E27" s="11"/>
       <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
+      <c r="G27" s="20"/>
       <c r="H27" s="12"/>
       <c r="I27"/>
       <c r="J27"/>
@@ -2470,16 +2446,20 @@
     </row>
     <row r="28" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A28" s="6" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="11"/>
+      <c r="C28" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" s="18"/>
       <c r="E28" s="11"/>
       <c r="F28" s="11"/>
-      <c r="G28" s="21"/>
+      <c r="G28" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="H28" s="12"/>
       <c r="I28"/>
       <c r="J28"/>
@@ -2517,23 +2497,17 @@
       <c r="AP28"/>
       <c r="AQ28"/>
     </row>
-    <row r="29" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A29" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B29" s="5" t="s">
+    <row r="29" spans="1:43" s="2" customFormat="1" ht="30.5" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="A29" s="7"/>
+      <c r="B29" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="C29" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="D29" s="18"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="H29" s="12"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="14"/>
       <c r="I29"/>
       <c r="J29"/>
       <c r="K29"/>
@@ -2570,51 +2544,7 @@
       <c r="AP29"/>
       <c r="AQ29"/>
     </row>
-    <row r="30" spans="1:43" s="2" customFormat="1" ht="30.5" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A30" s="7"/>
-      <c r="B30" s="22"/>
-      <c r="C30" s="23"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="23"/>
-      <c r="H30" s="14"/>
-      <c r="I30"/>
-      <c r="J30"/>
-      <c r="K30"/>
-      <c r="L30"/>
-      <c r="M30"/>
-      <c r="N30"/>
-      <c r="O30"/>
-      <c r="P30"/>
-      <c r="Q30"/>
-      <c r="R30"/>
-      <c r="S30"/>
-      <c r="T30"/>
-      <c r="U30"/>
-      <c r="V30"/>
-      <c r="W30"/>
-      <c r="X30"/>
-      <c r="Y30"/>
-      <c r="Z30"/>
-      <c r="AA30"/>
-      <c r="AB30"/>
-      <c r="AC30"/>
-      <c r="AD30"/>
-      <c r="AE30"/>
-      <c r="AF30"/>
-      <c r="AG30"/>
-      <c r="AH30"/>
-      <c r="AI30"/>
-      <c r="AJ30"/>
-      <c r="AK30"/>
-      <c r="AL30"/>
-      <c r="AM30"/>
-      <c r="AN30"/>
-      <c r="AO30"/>
-      <c r="AP30"/>
-      <c r="AQ30"/>
-    </row>
+    <row r="30" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="31" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="32" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="33" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -2660,14 +2590,13 @@
     <row r="73" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="74" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="75" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="76" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="A25:H25"/>
+    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="A24:H24"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
     <mergeCell ref="G1:H1"/>

</xml_diff>

<commit_message>
documentation ajout ap2 putty tableau de synthese
</commit_message>
<xml_diff>
--- a/public/assets/- Tableau de synthèse - Epreuve E4 - BTS SIO 2025.xlsx
+++ b/public/assets/- Tableau de synthèse - Epreuve E4 - BTS SIO 2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ymokhtari\portfolio\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{939FD3F7-7FFF-4E31-87AE-6ED889937F69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E2826FF-21E1-43CB-92F2-2C998E11DDB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Tableau de synthèse Épreuve E4" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Tableau de synthèse Épreuve E4'!$A$1:$H$29</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Tableau de synthèse Épreuve E4'!$A$1:$H$28</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="54">
   <si>
     <t>BTS SERVICES INFORMATIQUES AUX ORGANISATIONS</t>
   </si>
@@ -144,51 +144,27 @@
     <t>X</t>
   </si>
   <si>
-    <t>du 27/10/2023 au 29/10/2023</t>
-  </si>
-  <si>
-    <t>du 27/05/2024 au 05/07/2024</t>
-  </si>
-  <si>
-    <t>du 02/09/2024 au 18/07/2025</t>
-  </si>
-  <si>
     <t>Creation d'entreprise virtuelle (AP1)</t>
   </si>
   <si>
     <t>Installation et configuration d'un Hyperviseur Proxmox VE</t>
   </si>
   <si>
-    <t>du 30/09/2024 au 14/10/2024</t>
-  </si>
-  <si>
     <t>Installation et configuration d’un outil d’inventaire et ticketing (GLPI)</t>
   </si>
   <si>
     <t>Mettre en place un outil de veille technologique (Feedly, Google Alerts)</t>
   </si>
   <si>
-    <t>du 19/10/2024 au 02/11/2024</t>
-  </si>
-  <si>
     <t>Répondre aux problématique M2L (AP2)</t>
   </si>
   <si>
-    <t>du XX/XX/XXXX au XX/XX/XXXX</t>
-  </si>
-  <si>
     <t>Gestion des utilisateurs dans l’Active Directory</t>
   </si>
   <si>
     <t>Installation et configurations de postes pour les utilisateurs</t>
   </si>
   <si>
-    <t>Installation et configuration d'un Windows serveur 2022 AD</t>
-  </si>
-  <si>
-    <t>du 28/10/2024 au 04/11/2024</t>
-  </si>
-  <si>
     <t>Création d'un cron pour les actions automatiques GLPI</t>
   </si>
   <si>
@@ -214,6 +190,36 @@
   </si>
   <si>
     <t>Mise une place d'une Machine Virtuelle (Windows 10)</t>
+  </si>
+  <si>
+    <t>du 31/11/23 au 22/12/23</t>
+  </si>
+  <si>
+    <t>du 17/02/24 au 28/05/24</t>
+  </si>
+  <si>
+    <t>du 17/11/23 au 20/11/23</t>
+  </si>
+  <si>
+    <t>du 30/09/24 au 14/10/24</t>
+  </si>
+  <si>
+    <t>du 01/12/24 au 10/12/24</t>
+  </si>
+  <si>
+    <t>du 28/10/24 au 04/11/24</t>
+  </si>
+  <si>
+    <t>du 19/10/24 au 02/11/24</t>
+  </si>
+  <si>
+    <t>du 27/10/23 au 29/10/23</t>
+  </si>
+  <si>
+    <t>du 27/05/24 au 05/07/24</t>
+  </si>
+  <si>
+    <t>du 02/09/24 au 18/07/25</t>
   </si>
 </sst>
 </file>
@@ -1261,10 +1267,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AQ75"/>
+  <dimension ref="A1:AQ74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.90625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1311,7 +1317,7 @@
       <c r="D3" s="38"/>
       <c r="E3" s="39"/>
       <c r="F3" s="43" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="G3" s="38"/>
       <c r="H3" s="44"/>
@@ -1481,10 +1487,10 @@
     </row>
     <row r="9" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A9" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="11"/>
@@ -1534,10 +1540,10 @@
     </row>
     <row r="10" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A10" s="6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
@@ -1585,17 +1591,15 @@
     </row>
     <row r="11" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A11" s="6" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C11" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="18" t="s">
-        <v>27</v>
-      </c>
+      <c r="D11" s="11"/>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
       <c r="G11" s="18" t="s">
@@ -1640,10 +1644,10 @@
     </row>
     <row r="12" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A12" s="6" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="C12" s="18" t="s">
         <v>27</v>
@@ -1693,17 +1697,19 @@
     </row>
     <row r="13" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A13" s="6" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="C13" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="11"/>
+      <c r="D13" s="18"/>
       <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
+      <c r="F13" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="G13" s="18" t="s">
         <v>27</v>
       </c>
@@ -1746,20 +1752,18 @@
     </row>
     <row r="14" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A14" s="6" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="18"/>
       <c r="E14" s="11"/>
-      <c r="F14" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="G14" s="18" t="s">
+      <c r="F14" s="11"/>
+      <c r="G14" s="20" t="s">
         <v>27</v>
       </c>
       <c r="H14" s="12"/>
@@ -1799,23 +1803,21 @@
       <c r="AP14"/>
       <c r="AQ14"/>
     </row>
-    <row r="15" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="15" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="C15" s="11"/>
-      <c r="D15" s="18" t="s">
-        <v>27</v>
-      </c>
+      <c r="D15" s="11"/>
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
-      <c r="G15" s="20" t="s">
+      <c r="G15" s="11"/>
+      <c r="H15" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="H15" s="12"/>
       <c r="I15"/>
       <c r="J15"/>
       <c r="K15"/>
@@ -1854,10 +1856,10 @@
     </row>
     <row r="16" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
@@ -1903,21 +1905,17 @@
       <c r="AP16"/>
       <c r="AQ16"/>
     </row>
-    <row r="17" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="19" t="s">
-        <v>27</v>
-      </c>
+    <row r="17" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A17" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="30"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="31"/>
       <c r="I17"/>
       <c r="J17"/>
       <c r="K17"/>
@@ -1954,17 +1952,21 @@
       <c r="AP17"/>
       <c r="AQ17"/>
     </row>
-    <row r="18" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A18" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="30"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="30"/>
-      <c r="H18" s="31"/>
+    <row r="18" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A18" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="12"/>
       <c r="I18"/>
       <c r="J18"/>
       <c r="K18"/>
@@ -2003,15 +2005,17 @@
     </row>
     <row r="19" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A19" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="C19" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="11"/>
+      <c r="D19" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="E19" s="11"/>
       <c r="F19" s="11"/>
       <c r="G19" s="11"/>
@@ -2054,20 +2058,17 @@
     </row>
     <row r="20" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A20" s="6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="11"/>
+      <c r="G20" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
       <c r="H20" s="12"/>
       <c r="I20"/>
       <c r="J20"/>
@@ -2107,17 +2108,18 @@
     </row>
     <row r="21" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A21" s="6" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
+        <v>52</v>
+      </c>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
       <c r="E21" s="11"/>
-      <c r="G21" s="18" t="s">
+      <c r="F21" s="18" t="s">
         <v>27</v>
       </c>
+      <c r="G21" s="18"/>
       <c r="H21" s="12"/>
       <c r="I21"/>
       <c r="J21"/>
@@ -2156,19 +2158,13 @@
       <c r="AQ21"/>
     </row>
     <row r="22" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A22" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
+      <c r="A22" s="6"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
       <c r="E22" s="11"/>
-      <c r="F22" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="G22" s="18"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
       <c r="H22" s="12"/>
       <c r="I22"/>
       <c r="J22"/>
@@ -2206,15 +2202,17 @@
       <c r="AP22"/>
       <c r="AQ22"/>
     </row>
-    <row r="23" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A23" s="6"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="12"/>
+    <row r="23" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A23" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="30"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="30"/>
+      <c r="H23" s="31"/>
       <c r="I23"/>
       <c r="J23"/>
       <c r="K23"/>
@@ -2251,17 +2249,23 @@
       <c r="AP23"/>
       <c r="AQ23"/>
     </row>
-    <row r="24" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A24" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="B24" s="30"/>
-      <c r="C24" s="30"/>
-      <c r="D24" s="30"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="30"/>
-      <c r="G24" s="30"/>
-      <c r="H24" s="31"/>
+    <row r="24" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A24" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="12"/>
       <c r="I24"/>
       <c r="J24"/>
       <c r="K24"/>
@@ -2300,20 +2304,20 @@
     </row>
     <row r="25" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A25" s="6" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="C25" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="18" t="s">
-        <v>27</v>
-      </c>
+      <c r="D25" s="18"/>
       <c r="E25" s="11"/>
       <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
+      <c r="G25" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="H25" s="12"/>
       <c r="I25"/>
       <c r="J25"/>
@@ -2353,20 +2357,18 @@
     </row>
     <row r="26" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A26" s="6" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="C26" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D26" s="18"/>
+      <c r="D26" s="11"/>
       <c r="E26" s="11"/>
       <c r="F26" s="11"/>
-      <c r="G26" s="18" t="s">
-        <v>27</v>
-      </c>
+      <c r="G26" s="20"/>
       <c r="H26" s="12"/>
       <c r="I26"/>
       <c r="J26"/>
@@ -2406,18 +2408,20 @@
     </row>
     <row r="27" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A27" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="C27" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D27" s="11"/>
+      <c r="D27" s="18"/>
       <c r="E27" s="11"/>
       <c r="F27" s="11"/>
-      <c r="G27" s="20"/>
+      <c r="G27" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="H27" s="12"/>
       <c r="I27"/>
       <c r="J27"/>
@@ -2455,23 +2459,15 @@
       <c r="AP27"/>
       <c r="AQ27"/>
     </row>
-    <row r="28" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A28" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C28" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="D28" s="18"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="H28" s="12"/>
+    <row r="28" spans="1:43" s="2" customFormat="1" ht="30.5" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="A28" s="7"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="14"/>
       <c r="I28"/>
       <c r="J28"/>
       <c r="K28"/>
@@ -2508,53 +2504,7 @@
       <c r="AP28"/>
       <c r="AQ28"/>
     </row>
-    <row r="29" spans="1:43" s="2" customFormat="1" ht="30.5" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A29" s="7"/>
-      <c r="B29" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="C29" s="22"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="22"/>
-      <c r="H29" s="14"/>
-      <c r="I29"/>
-      <c r="J29"/>
-      <c r="K29"/>
-      <c r="L29"/>
-      <c r="M29"/>
-      <c r="N29"/>
-      <c r="O29"/>
-      <c r="P29"/>
-      <c r="Q29"/>
-      <c r="R29"/>
-      <c r="S29"/>
-      <c r="T29"/>
-      <c r="U29"/>
-      <c r="V29"/>
-      <c r="W29"/>
-      <c r="X29"/>
-      <c r="Y29"/>
-      <c r="Z29"/>
-      <c r="AA29"/>
-      <c r="AB29"/>
-      <c r="AC29"/>
-      <c r="AD29"/>
-      <c r="AE29"/>
-      <c r="AF29"/>
-      <c r="AG29"/>
-      <c r="AH29"/>
-      <c r="AI29"/>
-      <c r="AJ29"/>
-      <c r="AK29"/>
-      <c r="AL29"/>
-      <c r="AM29"/>
-      <c r="AN29"/>
-      <c r="AO29"/>
-      <c r="AP29"/>
-      <c r="AQ29"/>
-    </row>
+    <row r="29" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="31" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="32" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -2600,7 +2550,6 @@
     <row r="72" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="73" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="74" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="75" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
     <mergeCell ref="G1:H1"/>
@@ -2611,8 +2560,8 @@
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A18:H18"/>
-    <mergeCell ref="A24:H24"/>
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="A23:H23"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
   </mergeCells>

</xml_diff>